<commit_message>
Metiendo el documento y en blanco
</commit_message>
<xml_diff>
--- a/Validación.xlsx
+++ b/Validación.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="11070"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="11070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -264,13 +264,13 @@
     <t>En la selección del tipo de tarjeta</t>
   </si>
   <si>
-    <t>Podría ser interesante incluir paginación para las transferencias</t>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -675,11 +675,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C31" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>